<commit_message>
update: <AdminSection Module datepickerUtil added>
</commit_message>
<xml_diff>
--- a/src/main/resources/Config/TestData.xlsx
+++ b/src/main/resources/Config/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://provanaindia-my.sharepoint.com/personal/abhishek_kumar_provana_com1/Documents/Ipacs_Automation/ipacsQA/src/main/resources/Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="11_F25DC773A252ABDACC104891111D6FE65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB731A17-0E62-47DD-A9CF-68696E0478D8}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="11_F25DC773A252ABDACC104891111D6FE65ADE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53C590DA-A04C-4F79-A4F4-376730D5A4B4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -203,19 +203,19 @@
     <t>yes</t>
   </si>
   <si>
-    <t>testuser001@test.com</t>
-  </si>
-  <si>
     <t>Testuser</t>
   </si>
   <si>
     <t>EditUserName</t>
   </si>
   <si>
-    <t>Ecm04_testuser</t>
-  </si>
-  <si>
-    <t>Ecm04</t>
+    <t>Ecm06</t>
+  </si>
+  <si>
+    <t>Ecm06_testuser</t>
+  </si>
+  <si>
+    <t>testuser006@test.com</t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
   <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,7 +776,7 @@
         <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -784,7 +784,7 @@
         <v>46</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -800,7 +800,7 @@
         <v>48</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -845,7 +845,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B41" t="s">
         <v>58</v>

</xml_diff>